<commit_message>
Changes done to accomodate small summary in excel on what basis decision was agreed. Journal already had the details.
</commit_message>
<xml_diff>
--- a/Solid Principle Exercise Part 2/heuristics_2.x(combined) filled.xlsx
+++ b/Solid Principle Exercise Part 2/heuristics_2.x(combined) filled.xlsx
@@ -5,10 +5,10 @@
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vivek\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vivek\UCD\Studies\Design Pattern\Github\Solid Principle Exercise Part 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B33C9291-6AF7-4053-A934-A92343A132FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{733C7FC2-8454-4BC5-8A86-7135989F2D97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="103">
   <si>
     <t>Heuristic #2.1</t>
   </si>
@@ -256,9 +256,6 @@
     <t>ISP is 4.Abstraction of relevant things and not all necessary details of the role of object in program like Hashcode in Java should not be abstracted.</t>
   </si>
   <si>
-    <t>Encapsulation is part of SRP</t>
-  </si>
-  <si>
     <t>All are rated as 1 because we feel its about cyclic dependencies principle</t>
   </si>
   <si>
@@ -272,6 +269,90 @@
   </si>
   <si>
     <t>No keys about dependency abstraction</t>
+  </si>
+  <si>
+    <t>Encapsulation is part of SRP,Ru disagree.</t>
+  </si>
+  <si>
+    <t>No difference</t>
+  </si>
+  <si>
+    <t>A-1</t>
+  </si>
+  <si>
+    <t>A-5</t>
+  </si>
+  <si>
+    <t>Principle: Cyclic Dependecy</t>
+  </si>
+  <si>
+    <t>Principle: Cyclic Dependency</t>
+  </si>
+  <si>
+    <t>Somewhat related to reducing on need basis</t>
+  </si>
+  <si>
+    <t>Doesn't speak about what to modify and what not, rather when to modify.</t>
+  </si>
+  <si>
+    <t>Doesn't speak about inheritance</t>
+  </si>
+  <si>
+    <t>Doesn't speak about hiding unwanted implementation</t>
+  </si>
+  <si>
+    <t>No relation with responsibility</t>
+  </si>
+  <si>
+    <t>Client dependency on public interface</t>
+  </si>
+  <si>
+    <t>no relation</t>
+  </si>
+  <si>
+    <t>client shoul d not implement empty methods</t>
+  </si>
+  <si>
+    <t>No relation with what to modify and what to extend</t>
+  </si>
+  <si>
+    <t>No relation with inheritance</t>
+  </si>
+  <si>
+    <t>Interface belongs to client, keep it useful</t>
+  </si>
+  <si>
+    <t>Interface belongs to client, client doesn't need to work on what to</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No relation with inheritance </t>
+  </si>
+  <si>
+    <t>Dependency on public interface/client must override all methods of interface</t>
+  </si>
+  <si>
+    <t>No relation with what goes into interface</t>
+  </si>
+  <si>
+    <t>Speaks about single resposnibility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No relation with what to modify and what to extend </t>
+  </si>
+  <si>
+    <t>No relation with interface contents</t>
+  </si>
+  <si>
+    <t>No relation with what must be open and what must be close</t>
+  </si>
+  <si>
+    <t>No effect on resposnibility</t>
+  </si>
+  <si>
+    <t>Speaks about inhertiance but more on how to create class and categorize the objects by attribute and not role</t>
+  </si>
+  <si>
+    <t>No relation with call heirarchy</t>
   </si>
 </sst>
 </file>
@@ -585,12 +666,6 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -629,6 +704,12 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
@@ -1119,8 +1200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="R12" workbookViewId="0">
+      <selection activeCell="AG6" sqref="AG6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1172,10 +1253,10 @@
       <c r="F1" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="28" t="s">
         <v>40</v>
       </c>
       <c r="I1" s="5" t="s">
@@ -1190,10 +1271,10 @@
       <c r="L1" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="M1" s="22" t="s">
+      <c r="M1" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="N1" s="15" t="s">
+      <c r="N1" s="28" t="s">
         <v>40</v>
       </c>
       <c r="O1" s="5" t="s">
@@ -1208,10 +1289,10 @@
       <c r="R1" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="S1" s="22" t="s">
+      <c r="S1" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="T1" s="15" t="s">
+      <c r="T1" s="28" t="s">
         <v>40</v>
       </c>
       <c r="U1" s="5" t="s">
@@ -1226,10 +1307,10 @@
       <c r="X1" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="Y1" s="22" t="s">
+      <c r="Y1" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="Z1" s="15" t="s">
+      <c r="Z1" s="28" t="s">
         <v>40</v>
       </c>
       <c r="AA1" s="5" t="s">
@@ -1244,14 +1325,14 @@
       <c r="AD1" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="AE1" s="22" t="s">
+      <c r="AE1" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="AF1" s="15" t="s">
+      <c r="AF1" s="28" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:33" ht="54" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:33" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1274,11 +1355,11 @@
         <f>'Ruyue Jin'!C2</f>
         <v>1</v>
       </c>
-      <c r="G2" s="23" t="s">
+      <c r="G2" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="H2" s="28" t="s">
-        <v>70</v>
+      <c r="H2" s="26" t="s">
+        <v>75</v>
       </c>
       <c r="I2" s="7">
         <f>AVERAGE('Vivek Murarka'!D2, 'Ruyue Jin'!D2)</f>
@@ -1296,8 +1377,12 @@
         <f>'Ruyue Jin'!D2</f>
         <v>1</v>
       </c>
-      <c r="M2" s="23"/>
-      <c r="N2" s="16"/>
+      <c r="M2" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="N2" s="29" t="s">
+        <v>76</v>
+      </c>
       <c r="O2" s="7">
         <f>AVERAGE('Vivek Murarka'!E2, 'Ruyue Jin'!E2)</f>
         <v>1</v>
@@ -1314,8 +1399,12 @@
         <f>'Ruyue Jin'!E2</f>
         <v>1</v>
       </c>
-      <c r="S2" s="23"/>
-      <c r="T2" s="16"/>
+      <c r="S2" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="T2" s="29" t="s">
+        <v>76</v>
+      </c>
       <c r="U2" s="7">
         <f>AVERAGE('Vivek Murarka'!F2, 'Ruyue Jin'!F2)</f>
         <v>1</v>
@@ -1332,8 +1421,12 @@
         <f>'Ruyue Jin'!F2</f>
         <v>1</v>
       </c>
-      <c r="Y2" s="23"/>
-      <c r="Z2" s="16"/>
+      <c r="Y2" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z2" s="29" t="s">
+        <v>76</v>
+      </c>
       <c r="AA2" s="7">
         <f>AVERAGE('Vivek Murarka'!G2, 'Ruyue Jin'!G2)</f>
         <v>1</v>
@@ -1350,10 +1443,14 @@
         <f>'Ruyue Jin'!G2</f>
         <v>1</v>
       </c>
-      <c r="AE2" s="23"/>
-      <c r="AF2" s="16"/>
-    </row>
-    <row r="3" spans="1:33" ht="36" x14ac:dyDescent="0.3">
+      <c r="AE2" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF2" s="29" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -1376,10 +1473,12 @@
         <f>'Ruyue Jin'!C3</f>
         <v>5</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="G3" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="H3" s="16"/>
+      <c r="H3" s="29" t="s">
+        <v>80</v>
+      </c>
       <c r="I3" s="7">
         <f>AVERAGE('Vivek Murarka'!D3, 'Ruyue Jin'!D3)</f>
         <v>3</v>
@@ -1396,10 +1495,12 @@
         <f>'Ruyue Jin'!D3</f>
         <v>1</v>
       </c>
-      <c r="M3" s="23" t="s">
+      <c r="M3" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="N3" s="16"/>
+      <c r="N3" s="29" t="s">
+        <v>80</v>
+      </c>
       <c r="O3" s="7">
         <f>AVERAGE('Vivek Murarka'!E3, 'Ruyue Jin'!E3)</f>
         <v>1</v>
@@ -1416,8 +1517,12 @@
         <f>'Ruyue Jin'!E3</f>
         <v>1</v>
       </c>
-      <c r="S3" s="23"/>
-      <c r="T3" s="16"/>
+      <c r="S3" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="T3" s="29" t="s">
+        <v>80</v>
+      </c>
       <c r="U3" s="7">
         <f>AVERAGE('Vivek Murarka'!F3, 'Ruyue Jin'!F3)</f>
         <v>1</v>
@@ -1434,8 +1539,12 @@
         <f>'Ruyue Jin'!F3</f>
         <v>1</v>
       </c>
-      <c r="Y3" s="23"/>
-      <c r="Z3" s="16"/>
+      <c r="Y3" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z3" s="29" t="s">
+        <v>80</v>
+      </c>
       <c r="AA3" s="7">
         <f>AVERAGE('Vivek Murarka'!G3, 'Ruyue Jin'!G3)</f>
         <v>2.5</v>
@@ -1452,15 +1561,17 @@
         <f>'Ruyue Jin'!G3</f>
         <v>1</v>
       </c>
-      <c r="AE3" s="23" t="s">
+      <c r="AE3" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="AF3" s="16"/>
-      <c r="AG3" s="29" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:33" ht="18" x14ac:dyDescent="0.3">
+      <c r="AF3" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="AG3" s="27" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" ht="126" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
@@ -1483,10 +1594,12 @@
         <f>'Ruyue Jin'!C4</f>
         <v>1</v>
       </c>
-      <c r="G4" s="23" t="s">
+      <c r="G4" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="H4" s="16"/>
+      <c r="H4" s="29" t="s">
+        <v>81</v>
+      </c>
       <c r="I4" s="7">
         <f>AVERAGE('Vivek Murarka'!D4, 'Ruyue Jin'!D4)</f>
         <v>3</v>
@@ -1503,10 +1616,12 @@
         <f>'Ruyue Jin'!D4</f>
         <v>5</v>
       </c>
-      <c r="M4" s="23" t="s">
+      <c r="M4" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="N4" s="16"/>
+      <c r="N4" s="29" t="s">
+        <v>82</v>
+      </c>
       <c r="O4" s="7">
         <f>AVERAGE('Vivek Murarka'!E4, 'Ruyue Jin'!E4)</f>
         <v>3</v>
@@ -1523,10 +1638,12 @@
         <f>'Ruyue Jin'!E4</f>
         <v>1</v>
       </c>
-      <c r="S4" s="23" t="s">
+      <c r="S4" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="T4" s="16"/>
+      <c r="T4" s="29" t="s">
+        <v>83</v>
+      </c>
       <c r="U4" s="7">
         <f>AVERAGE('Vivek Murarka'!F4, 'Ruyue Jin'!F4)</f>
         <v>2</v>
@@ -1543,10 +1660,12 @@
         <f>'Ruyue Jin'!F4</f>
         <v>3</v>
       </c>
-      <c r="Y4" s="23" t="s">
+      <c r="Y4" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="Z4" s="16"/>
+      <c r="Z4" s="29" t="s">
+        <v>84</v>
+      </c>
       <c r="AA4" s="7">
         <f>AVERAGE('Vivek Murarka'!G4, 'Ruyue Jin'!G4)</f>
         <v>1.5</v>
@@ -1563,12 +1682,14 @@
         <f>'Ruyue Jin'!G4</f>
         <v>1</v>
       </c>
-      <c r="AE4" s="23" t="s">
+      <c r="AE4" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="AF4" s="16"/>
-    </row>
-    <row r="5" spans="1:33" ht="36" x14ac:dyDescent="0.3">
+      <c r="AF4" s="29" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" ht="108" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
@@ -1591,10 +1712,12 @@
         <f>'Ruyue Jin'!C5</f>
         <v>1</v>
       </c>
-      <c r="G5" s="23" t="s">
+      <c r="G5" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="H5" s="16"/>
+      <c r="H5" s="29" t="s">
+        <v>85</v>
+      </c>
       <c r="I5" s="7">
         <f>AVERAGE('Vivek Murarka'!D5, 'Ruyue Jin'!D5)</f>
         <v>4</v>
@@ -1611,10 +1734,12 @@
         <f>'Ruyue Jin'!D5</f>
         <v>5</v>
       </c>
-      <c r="M5" s="23" t="s">
+      <c r="M5" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="N5" s="16"/>
+      <c r="N5" s="29" t="s">
+        <v>86</v>
+      </c>
       <c r="O5" s="7">
         <f>AVERAGE('Vivek Murarka'!E5, 'Ruyue Jin'!E5)</f>
         <v>1</v>
@@ -1631,8 +1756,12 @@
         <f>'Ruyue Jin'!E5</f>
         <v>1</v>
       </c>
-      <c r="S5" s="23"/>
-      <c r="T5" s="16"/>
+      <c r="S5" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="T5" s="29" t="s">
+        <v>87</v>
+      </c>
       <c r="U5" s="7">
         <f>AVERAGE('Vivek Murarka'!F5, 'Ruyue Jin'!F5)</f>
         <v>3</v>
@@ -1649,10 +1778,12 @@
         <f>'Ruyue Jin'!F5</f>
         <v>1</v>
       </c>
-      <c r="Y5" s="23" t="s">
+      <c r="Y5" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="Z5" s="16"/>
+      <c r="Z5" s="29" t="s">
+        <v>88</v>
+      </c>
       <c r="AA5" s="7">
         <f>AVERAGE('Vivek Murarka'!G5, 'Ruyue Jin'!G5)</f>
         <v>1</v>
@@ -1669,10 +1800,14 @@
         <f>'Ruyue Jin'!G5</f>
         <v>1</v>
       </c>
-      <c r="AE5" s="23"/>
-      <c r="AF5" s="16"/>
-    </row>
-    <row r="6" spans="1:33" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="AE5" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF5" s="29" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" ht="144" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
@@ -1695,8 +1830,12 @@
         <f>'Ruyue Jin'!C6</f>
         <v>1</v>
       </c>
-      <c r="G6" s="23"/>
-      <c r="H6" s="16"/>
+      <c r="G6" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="H6" s="29" t="s">
+        <v>85</v>
+      </c>
       <c r="I6" s="7">
         <f>AVERAGE('Vivek Murarka'!D6, 'Ruyue Jin'!D6)</f>
         <v>1.5</v>
@@ -1713,10 +1852,12 @@
         <f>'Ruyue Jin'!D6</f>
         <v>1</v>
       </c>
-      <c r="M6" s="23" t="s">
+      <c r="M6" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="N6" s="16"/>
+      <c r="N6" s="29" t="s">
+        <v>89</v>
+      </c>
       <c r="O6" s="7">
         <f>AVERAGE('Vivek Murarka'!E6, 'Ruyue Jin'!E6)</f>
         <v>1</v>
@@ -1733,8 +1874,12 @@
         <f>'Ruyue Jin'!E6</f>
         <v>1</v>
       </c>
-      <c r="S6" s="23"/>
-      <c r="T6" s="16"/>
+      <c r="S6" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="T6" s="29" t="s">
+        <v>83</v>
+      </c>
       <c r="U6" s="7">
         <f>AVERAGE('Vivek Murarka'!F6, 'Ruyue Jin'!F6)</f>
         <v>4.5</v>
@@ -1751,10 +1896,12 @@
         <f>'Ruyue Jin'!F6</f>
         <v>5</v>
       </c>
-      <c r="Y6" s="23" t="s">
+      <c r="Y6" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="Z6" s="16"/>
+      <c r="Z6" s="29" t="s">
+        <v>92</v>
+      </c>
       <c r="AA6" s="7">
         <f>AVERAGE('Vivek Murarka'!G6, 'Ruyue Jin'!G6)</f>
         <v>3</v>
@@ -1771,14 +1918,14 @@
         <f>'Ruyue Jin'!G6</f>
         <v>1</v>
       </c>
-      <c r="AE6" s="23" t="s">
+      <c r="AE6" s="21" t="s">
         <v>57</v>
       </c>
       <c r="AF6" s="30" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:33" ht="36" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" ht="108" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
@@ -1801,8 +1948,12 @@
         <f>'Ruyue Jin'!C7</f>
         <v>1</v>
       </c>
-      <c r="G7" s="23"/>
-      <c r="H7" s="16"/>
+      <c r="G7" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="H7" s="29" t="s">
+        <v>85</v>
+      </c>
       <c r="I7" s="7">
         <f>AVERAGE('Vivek Murarka'!D7, 'Ruyue Jin'!D7)</f>
         <v>2.5</v>
@@ -1819,10 +1970,12 @@
         <f>'Ruyue Jin'!D7</f>
         <v>1</v>
       </c>
-      <c r="M7" s="23" t="s">
+      <c r="M7" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="N7" s="16"/>
+      <c r="N7" s="29" t="s">
+        <v>89</v>
+      </c>
       <c r="O7" s="7">
         <f>AVERAGE('Vivek Murarka'!E7, 'Ruyue Jin'!E7)</f>
         <v>2</v>
@@ -1839,10 +1992,12 @@
         <f>'Ruyue Jin'!E7</f>
         <v>1</v>
       </c>
-      <c r="S7" s="23" t="s">
+      <c r="S7" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="T7" s="16"/>
+      <c r="T7" s="29" t="s">
+        <v>90</v>
+      </c>
       <c r="U7" s="7">
         <f>AVERAGE('Vivek Murarka'!F7, 'Ruyue Jin'!F7)</f>
         <v>5</v>
@@ -1859,8 +2014,12 @@
         <f>'Ruyue Jin'!F7</f>
         <v>5</v>
       </c>
-      <c r="Y7" s="23"/>
-      <c r="Z7" s="16"/>
+      <c r="Y7" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z7" s="29" t="s">
+        <v>91</v>
+      </c>
       <c r="AA7" s="7">
         <f>AVERAGE('Vivek Murarka'!G7, 'Ruyue Jin'!G7)</f>
         <v>1</v>
@@ -1877,10 +2036,14 @@
         <f>'Ruyue Jin'!G7</f>
         <v>1</v>
       </c>
-      <c r="AE7" s="23"/>
-      <c r="AF7" s="16"/>
-    </row>
-    <row r="8" spans="1:33" ht="36" x14ac:dyDescent="0.3">
+      <c r="AE7" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF7" s="29" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" ht="126" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
@@ -1903,8 +2066,12 @@
         <f>'Ruyue Jin'!C8</f>
         <v>1</v>
       </c>
-      <c r="G8" s="23"/>
-      <c r="H8" s="16"/>
+      <c r="G8" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="H8" s="29" t="s">
+        <v>85</v>
+      </c>
       <c r="I8" s="7">
         <f>AVERAGE('Vivek Murarka'!D8, 'Ruyue Jin'!D8)</f>
         <v>5</v>
@@ -1921,8 +2088,12 @@
         <f>'Ruyue Jin'!D8</f>
         <v>5</v>
       </c>
-      <c r="M8" s="23"/>
-      <c r="N8" s="16"/>
+      <c r="M8" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="N8" s="29" t="s">
+        <v>94</v>
+      </c>
       <c r="O8" s="7">
         <f>AVERAGE('Vivek Murarka'!E8, 'Ruyue Jin'!E8)</f>
         <v>1</v>
@@ -1939,8 +2110,12 @@
         <f>'Ruyue Jin'!E8</f>
         <v>1</v>
       </c>
-      <c r="S8" s="23"/>
-      <c r="T8" s="16"/>
+      <c r="S8" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="T8" s="29" t="s">
+        <v>93</v>
+      </c>
       <c r="U8" s="7">
         <f>AVERAGE('Vivek Murarka'!F8, 'Ruyue Jin'!F8)</f>
         <v>2</v>
@@ -1957,10 +2132,12 @@
         <f>'Ruyue Jin'!F8</f>
         <v>3</v>
       </c>
-      <c r="Y8" s="23" t="s">
+      <c r="Y8" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="Z8" s="16"/>
+      <c r="Z8" s="29" t="s">
+        <v>95</v>
+      </c>
       <c r="AA8" s="7">
         <f>AVERAGE('Vivek Murarka'!G8, 'Ruyue Jin'!G8)</f>
         <v>1</v>
@@ -1977,10 +2154,14 @@
         <f>'Ruyue Jin'!G8</f>
         <v>1</v>
       </c>
-      <c r="AE8" s="23"/>
-      <c r="AF8" s="16"/>
-    </row>
-    <row r="9" spans="1:33" ht="18" x14ac:dyDescent="0.3">
+      <c r="AE8" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF8" s="29" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" ht="108" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
@@ -2003,8 +2184,12 @@
         <f>'Ruyue Jin'!C9</f>
         <v>5</v>
       </c>
-      <c r="G9" s="23"/>
-      <c r="H9" s="16"/>
+      <c r="G9" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="H9" s="29" t="s">
+        <v>96</v>
+      </c>
       <c r="I9" s="7">
         <f>AVERAGE('Vivek Murarka'!D9, 'Ruyue Jin'!D9)</f>
         <v>1</v>
@@ -2021,8 +2206,12 @@
         <f>'Ruyue Jin'!D9</f>
         <v>1</v>
       </c>
-      <c r="M9" s="23"/>
-      <c r="N9" s="16"/>
+      <c r="M9" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="N9" s="29" t="s">
+        <v>97</v>
+      </c>
       <c r="O9" s="7">
         <f>AVERAGE('Vivek Murarka'!E9, 'Ruyue Jin'!E9)</f>
         <v>1</v>
@@ -2039,8 +2228,12 @@
         <f>'Ruyue Jin'!E9</f>
         <v>1</v>
       </c>
-      <c r="S9" s="23"/>
-      <c r="T9" s="16"/>
+      <c r="S9" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="T9" s="29" t="s">
+        <v>90</v>
+      </c>
       <c r="U9" s="7">
         <f>AVERAGE('Vivek Murarka'!F9, 'Ruyue Jin'!F9)</f>
         <v>1</v>
@@ -2057,8 +2250,12 @@
         <f>'Ruyue Jin'!F9</f>
         <v>1</v>
       </c>
-      <c r="Y9" s="23"/>
-      <c r="Z9" s="16"/>
+      <c r="Y9" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z9" s="29" t="s">
+        <v>95</v>
+      </c>
       <c r="AA9" s="7">
         <f>AVERAGE('Vivek Murarka'!G9, 'Ruyue Jin'!G9)</f>
         <v>1</v>
@@ -2075,10 +2272,14 @@
         <f>'Ruyue Jin'!G9</f>
         <v>1</v>
       </c>
-      <c r="AE9" s="23"/>
-      <c r="AF9" s="16"/>
-    </row>
-    <row r="10" spans="1:33" ht="90" x14ac:dyDescent="0.3">
+      <c r="AE9" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF9" s="29" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" ht="108" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>11</v>
       </c>
@@ -2101,11 +2302,11 @@
         <f>'Ruyue Jin'!C10</f>
         <v>5</v>
       </c>
-      <c r="G10" s="23" t="s">
+      <c r="G10" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="H10" s="28" t="s">
-        <v>73</v>
+      <c r="H10" s="26" t="s">
+        <v>72</v>
       </c>
       <c r="I10" s="7">
         <f>AVERAGE('Vivek Murarka'!D10, 'Ruyue Jin'!D10)</f>
@@ -2123,8 +2324,12 @@
         <f>'Ruyue Jin'!D10</f>
         <v>1</v>
       </c>
-      <c r="M10" s="23"/>
-      <c r="N10" s="16"/>
+      <c r="M10" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="N10" s="29" t="s">
+        <v>99</v>
+      </c>
       <c r="O10" s="7">
         <f>AVERAGE('Vivek Murarka'!E10, 'Ruyue Jin'!E10)</f>
         <v>1</v>
@@ -2141,8 +2346,12 @@
         <f>'Ruyue Jin'!E10</f>
         <v>1</v>
       </c>
-      <c r="S10" s="23"/>
-      <c r="T10" s="16"/>
+      <c r="S10" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="T10" s="29" t="s">
+        <v>90</v>
+      </c>
       <c r="U10" s="7">
         <f>AVERAGE('Vivek Murarka'!F10, 'Ruyue Jin'!F10)</f>
         <v>1</v>
@@ -2159,8 +2368,12 @@
         <f>'Ruyue Jin'!F10</f>
         <v>1</v>
       </c>
-      <c r="Y10" s="23"/>
-      <c r="Z10" s="16"/>
+      <c r="Y10" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z10" s="29" t="s">
+        <v>98</v>
+      </c>
       <c r="AA10" s="7">
         <f>AVERAGE('Vivek Murarka'!G10, 'Ruyue Jin'!G10)</f>
         <v>1</v>
@@ -2177,10 +2390,14 @@
         <f>'Ruyue Jin'!G10</f>
         <v>1</v>
       </c>
-      <c r="AE10" s="23"/>
-      <c r="AF10" s="16"/>
-    </row>
-    <row r="11" spans="1:33" ht="54" x14ac:dyDescent="0.3">
+      <c r="AE10" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF10" s="29" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" ht="108" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
@@ -2203,11 +2420,11 @@
         <f>'Ruyue Jin'!C11</f>
         <v>5</v>
       </c>
-      <c r="G11" s="23" t="s">
+      <c r="G11" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="H11" s="28" t="s">
-        <v>74</v>
+      <c r="H11" s="26" t="s">
+        <v>73</v>
       </c>
       <c r="I11" s="7">
         <f>AVERAGE('Vivek Murarka'!D11, 'Ruyue Jin'!D11)</f>
@@ -2225,8 +2442,12 @@
         <f>'Ruyue Jin'!D11</f>
         <v>1</v>
       </c>
-      <c r="M11" s="23"/>
-      <c r="N11" s="16"/>
+      <c r="M11" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="N11" s="29" t="s">
+        <v>99</v>
+      </c>
       <c r="O11" s="7">
         <f>AVERAGE('Vivek Murarka'!E11, 'Ruyue Jin'!E11)</f>
         <v>1</v>
@@ -2243,8 +2464,12 @@
         <f>'Ruyue Jin'!E11</f>
         <v>1</v>
       </c>
-      <c r="S11" s="23"/>
-      <c r="T11" s="16"/>
+      <c r="S11" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="T11" s="29" t="s">
+        <v>90</v>
+      </c>
       <c r="U11" s="7">
         <f>AVERAGE('Vivek Murarka'!F11, 'Ruyue Jin'!F11)</f>
         <v>1</v>
@@ -2261,8 +2486,12 @@
         <f>'Ruyue Jin'!F11</f>
         <v>1</v>
       </c>
-      <c r="Y11" s="23"/>
-      <c r="Z11" s="16"/>
+      <c r="Y11" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z11" s="29" t="s">
+        <v>95</v>
+      </c>
       <c r="AA11" s="7">
         <f>AVERAGE('Vivek Murarka'!G11, 'Ruyue Jin'!G11)</f>
         <v>1</v>
@@ -2279,10 +2508,14 @@
         <f>'Ruyue Jin'!G11</f>
         <v>1</v>
       </c>
-      <c r="AE11" s="23"/>
-      <c r="AF11" s="16"/>
-    </row>
-    <row r="12" spans="1:33" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="AE11" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF11" s="29" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" ht="252" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>14</v>
       </c>
@@ -2305,8 +2538,12 @@
         <f>'Ruyue Jin'!C12</f>
         <v>1</v>
       </c>
-      <c r="G12" s="23"/>
-      <c r="H12" s="16"/>
+      <c r="G12" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="H12" s="29" t="s">
+        <v>100</v>
+      </c>
       <c r="I12" s="7">
         <f>AVERAGE('Vivek Murarka'!D12, 'Ruyue Jin'!D12)</f>
         <v>1</v>
@@ -2323,8 +2560,12 @@
         <f>'Ruyue Jin'!D12</f>
         <v>1</v>
       </c>
-      <c r="M12" s="23"/>
-      <c r="N12" s="16"/>
+      <c r="M12" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="N12" s="29" t="s">
+        <v>99</v>
+      </c>
       <c r="O12" s="7">
         <f>AVERAGE('Vivek Murarka'!E12, 'Ruyue Jin'!E12)</f>
         <v>1</v>
@@ -2341,8 +2582,12 @@
         <f>'Ruyue Jin'!E12</f>
         <v>1</v>
       </c>
-      <c r="S12" s="23"/>
-      <c r="T12" s="16"/>
+      <c r="S12" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="T12" s="29" t="s">
+        <v>101</v>
+      </c>
       <c r="U12" s="7">
         <f>AVERAGE('Vivek Murarka'!F12, 'Ruyue Jin'!F12)</f>
         <v>2.5</v>
@@ -2359,10 +2604,12 @@
         <f>'Ruyue Jin'!F12</f>
         <v>1</v>
       </c>
-      <c r="Y12" s="23" t="s">
+      <c r="Y12" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="Z12" s="16"/>
+      <c r="Z12" s="29" t="s">
+        <v>98</v>
+      </c>
       <c r="AA12" s="7">
         <f>AVERAGE('Vivek Murarka'!G12, 'Ruyue Jin'!G12)</f>
         <v>1.5</v>
@@ -2379,12 +2626,14 @@
         <f>'Ruyue Jin'!G12</f>
         <v>2</v>
       </c>
-      <c r="AE12" s="23" t="s">
+      <c r="AE12" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="AF12" s="16"/>
+      <c r="AF12" s="29" t="s">
+        <v>102</v>
+      </c>
       <c r="AG12" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:33" s="11" customFormat="1" ht="18" x14ac:dyDescent="0.35">
@@ -2443,8 +2692,8 @@
         <f>AVERAGE(R2:R12)</f>
         <v>1</v>
       </c>
-      <c r="S13" s="21"/>
-      <c r="T13" s="21"/>
+      <c r="S13" s="19"/>
+      <c r="T13" s="19"/>
       <c r="U13" s="5">
         <f>AVERAGE(U2:U12)</f>
         <v>2.1818181818181817</v>
@@ -2532,27 +2781,27 @@
       </c>
     </row>
     <row r="23" spans="2:2" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="B23" s="26" t="s">
+      <c r="B23" s="24" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="24" spans="2:2" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="B24" s="26" t="s">
+      <c r="B24" s="24" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B25" s="26" t="s">
+      <c r="B25" s="24" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B26" s="26" t="s">
+      <c r="B26" s="24" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="27" spans="2:2" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="B27" s="26" t="s">
+      <c r="B27" s="24" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2614,10 +2863,10 @@
       <c r="G1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="I1" s="15" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2628,25 +2877,25 @@
       <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="18">
-        <v>5</v>
-      </c>
-      <c r="D2" s="18">
-        <v>1</v>
-      </c>
-      <c r="E2" s="18">
-        <v>1</v>
-      </c>
-      <c r="F2" s="18">
-        <v>1</v>
-      </c>
-      <c r="G2" s="18">
-        <v>1</v>
-      </c>
-      <c r="H2" s="27" t="s">
+      <c r="C2" s="16">
+        <v>5</v>
+      </c>
+      <c r="D2" s="16">
+        <v>1</v>
+      </c>
+      <c r="E2" s="16">
+        <v>1</v>
+      </c>
+      <c r="F2" s="16">
+        <v>1</v>
+      </c>
+      <c r="G2" s="16">
+        <v>1</v>
+      </c>
+      <c r="H2" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="I2" s="20"/>
+      <c r="I2" s="18"/>
     </row>
     <row r="3" spans="1:9" ht="288" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
@@ -2655,25 +2904,25 @@
       <c r="B3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="18">
-        <v>1</v>
-      </c>
-      <c r="D3" s="18">
-        <v>5</v>
-      </c>
-      <c r="E3" s="18">
-        <v>1</v>
-      </c>
-      <c r="F3" s="18">
-        <v>1</v>
-      </c>
-      <c r="G3" s="18">
+      <c r="C3" s="16">
+        <v>1</v>
+      </c>
+      <c r="D3" s="16">
+        <v>5</v>
+      </c>
+      <c r="E3" s="16">
+        <v>1</v>
+      </c>
+      <c r="F3" s="16">
+        <v>1</v>
+      </c>
+      <c r="G3" s="16">
         <v>4</v>
       </c>
-      <c r="H3" s="27" t="s">
+      <c r="H3" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="I3" s="20"/>
+      <c r="I3" s="18"/>
     </row>
     <row r="4" spans="1:9" ht="90" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
@@ -2682,25 +2931,25 @@
       <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="18">
-        <v>1</v>
-      </c>
-      <c r="D4" s="18">
-        <v>1</v>
-      </c>
-      <c r="E4" s="18">
-        <v>5</v>
-      </c>
-      <c r="F4" s="18">
-        <v>1</v>
-      </c>
-      <c r="G4" s="18">
+      <c r="C4" s="16">
+        <v>1</v>
+      </c>
+      <c r="D4" s="16">
+        <v>1</v>
+      </c>
+      <c r="E4" s="16">
+        <v>5</v>
+      </c>
+      <c r="F4" s="16">
+        <v>1</v>
+      </c>
+      <c r="G4" s="16">
         <v>2</v>
       </c>
-      <c r="H4" s="27" t="s">
+      <c r="H4" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="I4" s="20"/>
+      <c r="I4" s="18"/>
     </row>
     <row r="5" spans="1:9" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
@@ -2709,25 +2958,25 @@
       <c r="B5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="16">
         <v>2</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="16">
         <v>3</v>
       </c>
-      <c r="E5" s="18">
-        <v>1</v>
-      </c>
-      <c r="F5" s="18">
-        <v>5</v>
-      </c>
-      <c r="G5" s="18">
-        <v>1</v>
-      </c>
-      <c r="H5" s="27" t="s">
+      <c r="E5" s="16">
+        <v>1</v>
+      </c>
+      <c r="F5" s="16">
+        <v>5</v>
+      </c>
+      <c r="G5" s="16">
+        <v>1</v>
+      </c>
+      <c r="H5" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="I5" s="20"/>
+      <c r="I5" s="18"/>
     </row>
     <row r="6" spans="1:9" ht="162" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
@@ -2736,25 +2985,25 @@
       <c r="B6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="18">
-        <v>1</v>
-      </c>
-      <c r="D6" s="18">
+      <c r="C6" s="16">
+        <v>1</v>
+      </c>
+      <c r="D6" s="16">
         <v>2</v>
       </c>
-      <c r="E6" s="18">
-        <v>1</v>
-      </c>
-      <c r="F6" s="18">
+      <c r="E6" s="16">
+        <v>1</v>
+      </c>
+      <c r="F6" s="16">
         <v>4</v>
       </c>
-      <c r="G6" s="18">
-        <v>5</v>
-      </c>
-      <c r="H6" s="27" t="s">
+      <c r="G6" s="16">
+        <v>5</v>
+      </c>
+      <c r="H6" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="I6" s="20"/>
+      <c r="I6" s="18"/>
     </row>
     <row r="7" spans="1:9" ht="126" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
@@ -2763,25 +3012,25 @@
       <c r="B7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="18">
-        <v>1</v>
-      </c>
-      <c r="D7" s="18">
+      <c r="C7" s="16">
+        <v>1</v>
+      </c>
+      <c r="D7" s="16">
         <v>4</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="16">
         <v>3</v>
       </c>
-      <c r="F7" s="18">
-        <v>5</v>
-      </c>
-      <c r="G7" s="18">
-        <v>1</v>
-      </c>
-      <c r="H7" s="27" t="s">
+      <c r="F7" s="16">
+        <v>5</v>
+      </c>
+      <c r="G7" s="16">
+        <v>1</v>
+      </c>
+      <c r="H7" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="I7" s="20"/>
+      <c r="I7" s="18"/>
     </row>
     <row r="8" spans="1:9" ht="90" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
@@ -2790,25 +3039,25 @@
       <c r="B8" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="18">
-        <v>1</v>
-      </c>
-      <c r="D8" s="18">
-        <v>5</v>
-      </c>
-      <c r="E8" s="18">
-        <v>1</v>
-      </c>
-      <c r="F8" s="18">
-        <v>1</v>
-      </c>
-      <c r="G8" s="18">
-        <v>1</v>
-      </c>
-      <c r="H8" s="27" t="s">
+      <c r="C8" s="16">
+        <v>1</v>
+      </c>
+      <c r="D8" s="16">
+        <v>5</v>
+      </c>
+      <c r="E8" s="16">
+        <v>1</v>
+      </c>
+      <c r="F8" s="16">
+        <v>1</v>
+      </c>
+      <c r="G8" s="16">
+        <v>1</v>
+      </c>
+      <c r="H8" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="I8" s="20"/>
+      <c r="I8" s="18"/>
     </row>
     <row r="9" spans="1:9" ht="54" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
@@ -2817,25 +3066,25 @@
       <c r="B9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="18">
-        <v>5</v>
-      </c>
-      <c r="D9" s="18">
-        <v>1</v>
-      </c>
-      <c r="E9" s="18">
-        <v>1</v>
-      </c>
-      <c r="F9" s="18">
-        <v>1</v>
-      </c>
-      <c r="G9" s="18">
-        <v>1</v>
-      </c>
-      <c r="H9" s="27" t="s">
+      <c r="C9" s="16">
+        <v>5</v>
+      </c>
+      <c r="D9" s="16">
+        <v>1</v>
+      </c>
+      <c r="E9" s="16">
+        <v>1</v>
+      </c>
+      <c r="F9" s="16">
+        <v>1</v>
+      </c>
+      <c r="G9" s="16">
+        <v>1</v>
+      </c>
+      <c r="H9" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="I9" s="20"/>
+      <c r="I9" s="18"/>
     </row>
     <row r="10" spans="1:9" ht="36" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
@@ -2844,25 +3093,25 @@
       <c r="B10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="18">
+      <c r="C10" s="16">
         <v>3</v>
       </c>
-      <c r="D10" s="18">
-        <v>1</v>
-      </c>
-      <c r="E10" s="18">
-        <v>1</v>
-      </c>
-      <c r="F10" s="18">
-        <v>1</v>
-      </c>
-      <c r="G10" s="18">
-        <v>1</v>
-      </c>
-      <c r="H10" s="27" t="s">
+      <c r="D10" s="16">
+        <v>1</v>
+      </c>
+      <c r="E10" s="16">
+        <v>1</v>
+      </c>
+      <c r="F10" s="16">
+        <v>1</v>
+      </c>
+      <c r="G10" s="16">
+        <v>1</v>
+      </c>
+      <c r="H10" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="I10" s="20"/>
+      <c r="I10" s="18"/>
     </row>
     <row r="11" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
@@ -2871,25 +3120,25 @@
       <c r="B11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="18">
-        <v>1</v>
-      </c>
-      <c r="D11" s="18">
-        <v>1</v>
-      </c>
-      <c r="E11" s="18">
-        <v>1</v>
-      </c>
-      <c r="F11" s="18">
-        <v>1</v>
-      </c>
-      <c r="G11" s="18">
-        <v>1</v>
-      </c>
-      <c r="H11" s="27" t="s">
+      <c r="C11" s="16">
+        <v>1</v>
+      </c>
+      <c r="D11" s="16">
+        <v>1</v>
+      </c>
+      <c r="E11" s="16">
+        <v>1</v>
+      </c>
+      <c r="F11" s="16">
+        <v>1</v>
+      </c>
+      <c r="G11" s="16">
+        <v>1</v>
+      </c>
+      <c r="H11" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="I11" s="20"/>
+      <c r="I11" s="18"/>
     </row>
     <row r="12" spans="1:9" ht="108" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
@@ -2898,25 +3147,25 @@
       <c r="B12" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="18">
-        <v>1</v>
-      </c>
-      <c r="D12" s="18">
-        <v>1</v>
-      </c>
-      <c r="E12" s="18">
-        <v>1</v>
-      </c>
-      <c r="F12" s="18">
+      <c r="C12" s="16">
+        <v>1</v>
+      </c>
+      <c r="D12" s="16">
+        <v>1</v>
+      </c>
+      <c r="E12" s="16">
+        <v>1</v>
+      </c>
+      <c r="F12" s="16">
         <v>4</v>
       </c>
-      <c r="G12" s="18">
-        <v>1</v>
-      </c>
-      <c r="H12" s="27" t="s">
+      <c r="G12" s="16">
+        <v>1</v>
+      </c>
+      <c r="H12" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="I12" s="20"/>
+      <c r="I12" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2972,10 +3221,10 @@
       <c r="G1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="I1" s="15" t="s">
         <v>21</v>
       </c>
       <c r="J1" s="2"/>
@@ -2987,23 +3236,23 @@
       <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="24">
-        <v>1</v>
-      </c>
-      <c r="D2" s="24">
-        <v>1</v>
-      </c>
-      <c r="E2" s="24">
-        <v>1</v>
-      </c>
-      <c r="F2" s="24">
-        <v>1</v>
-      </c>
-      <c r="G2" s="24">
-        <v>1</v>
-      </c>
-      <c r="H2" s="19"/>
-      <c r="I2" s="25" t="s">
+      <c r="C2" s="22">
+        <v>1</v>
+      </c>
+      <c r="D2" s="22">
+        <v>1</v>
+      </c>
+      <c r="E2" s="22">
+        <v>1</v>
+      </c>
+      <c r="F2" s="22">
+        <v>1</v>
+      </c>
+      <c r="G2" s="22">
+        <v>1</v>
+      </c>
+      <c r="H2" s="17"/>
+      <c r="I2" s="23" t="s">
         <v>47</v>
       </c>
     </row>
@@ -3014,23 +3263,23 @@
       <c r="B3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="24">
-        <v>5</v>
-      </c>
-      <c r="D3" s="24">
-        <v>1</v>
-      </c>
-      <c r="E3" s="24">
-        <v>1</v>
-      </c>
-      <c r="F3" s="24">
-        <v>1</v>
-      </c>
-      <c r="G3" s="24">
-        <v>1</v>
-      </c>
-      <c r="H3" s="19"/>
-      <c r="I3" s="25"/>
+      <c r="C3" s="22">
+        <v>5</v>
+      </c>
+      <c r="D3" s="22">
+        <v>1</v>
+      </c>
+      <c r="E3" s="22">
+        <v>1</v>
+      </c>
+      <c r="F3" s="22">
+        <v>1</v>
+      </c>
+      <c r="G3" s="22">
+        <v>1</v>
+      </c>
+      <c r="H3" s="17"/>
+      <c r="I3" s="23"/>
     </row>
     <row r="4" spans="1:10" ht="18" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
@@ -3039,23 +3288,23 @@
       <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="24">
-        <v>1</v>
-      </c>
-      <c r="D4" s="24">
-        <v>5</v>
-      </c>
-      <c r="E4" s="24">
-        <v>1</v>
-      </c>
-      <c r="F4" s="24">
+      <c r="C4" s="22">
+        <v>1</v>
+      </c>
+      <c r="D4" s="22">
+        <v>5</v>
+      </c>
+      <c r="E4" s="22">
+        <v>1</v>
+      </c>
+      <c r="F4" s="22">
         <v>3</v>
       </c>
-      <c r="G4" s="24">
-        <v>1</v>
-      </c>
-      <c r="H4" s="19"/>
-      <c r="I4" s="25"/>
+      <c r="G4" s="22">
+        <v>1</v>
+      </c>
+      <c r="H4" s="17"/>
+      <c r="I4" s="23"/>
     </row>
     <row r="5" spans="1:10" ht="54" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
@@ -3064,23 +3313,23 @@
       <c r="B5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="24">
-        <v>1</v>
-      </c>
-      <c r="D5" s="24">
-        <v>5</v>
-      </c>
-      <c r="E5" s="24">
-        <v>1</v>
-      </c>
-      <c r="F5" s="24">
-        <v>1</v>
-      </c>
-      <c r="G5" s="24">
-        <v>1</v>
-      </c>
-      <c r="H5" s="19"/>
-      <c r="I5" s="25"/>
+      <c r="C5" s="22">
+        <v>1</v>
+      </c>
+      <c r="D5" s="22">
+        <v>5</v>
+      </c>
+      <c r="E5" s="22">
+        <v>1</v>
+      </c>
+      <c r="F5" s="22">
+        <v>1</v>
+      </c>
+      <c r="G5" s="22">
+        <v>1</v>
+      </c>
+      <c r="H5" s="17"/>
+      <c r="I5" s="23"/>
     </row>
     <row r="6" spans="1:10" ht="36" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
@@ -3089,23 +3338,23 @@
       <c r="B6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="24">
-        <v>1</v>
-      </c>
-      <c r="D6" s="24">
-        <v>1</v>
-      </c>
-      <c r="E6" s="24">
-        <v>1</v>
-      </c>
-      <c r="F6" s="24">
-        <v>5</v>
-      </c>
-      <c r="G6" s="24">
-        <v>1</v>
-      </c>
-      <c r="H6" s="19"/>
-      <c r="I6" s="25"/>
+      <c r="C6" s="22">
+        <v>1</v>
+      </c>
+      <c r="D6" s="22">
+        <v>1</v>
+      </c>
+      <c r="E6" s="22">
+        <v>1</v>
+      </c>
+      <c r="F6" s="22">
+        <v>5</v>
+      </c>
+      <c r="G6" s="22">
+        <v>1</v>
+      </c>
+      <c r="H6" s="17"/>
+      <c r="I6" s="23"/>
     </row>
     <row r="7" spans="1:10" ht="36" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
@@ -3114,23 +3363,23 @@
       <c r="B7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="24">
-        <v>1</v>
-      </c>
-      <c r="D7" s="24">
-        <v>1</v>
-      </c>
-      <c r="E7" s="24">
-        <v>1</v>
-      </c>
-      <c r="F7" s="24">
-        <v>5</v>
-      </c>
-      <c r="G7" s="24">
-        <v>1</v>
-      </c>
-      <c r="H7" s="19"/>
-      <c r="I7" s="25"/>
+      <c r="C7" s="22">
+        <v>1</v>
+      </c>
+      <c r="D7" s="22">
+        <v>1</v>
+      </c>
+      <c r="E7" s="22">
+        <v>1</v>
+      </c>
+      <c r="F7" s="22">
+        <v>5</v>
+      </c>
+      <c r="G7" s="22">
+        <v>1</v>
+      </c>
+      <c r="H7" s="17"/>
+      <c r="I7" s="23"/>
     </row>
     <row r="8" spans="1:10" ht="54" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
@@ -3139,23 +3388,23 @@
       <c r="B8" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="24">
-        <v>1</v>
-      </c>
-      <c r="D8" s="24">
-        <v>5</v>
-      </c>
-      <c r="E8" s="24">
-        <v>1</v>
-      </c>
-      <c r="F8" s="24">
+      <c r="C8" s="22">
+        <v>1</v>
+      </c>
+      <c r="D8" s="22">
+        <v>5</v>
+      </c>
+      <c r="E8" s="22">
+        <v>1</v>
+      </c>
+      <c r="F8" s="22">
         <v>3</v>
       </c>
-      <c r="G8" s="24">
-        <v>1</v>
-      </c>
-      <c r="H8" s="19"/>
-      <c r="I8" s="25"/>
+      <c r="G8" s="22">
+        <v>1</v>
+      </c>
+      <c r="H8" s="17"/>
+      <c r="I8" s="23"/>
     </row>
     <row r="9" spans="1:10" ht="18" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
@@ -3164,23 +3413,23 @@
       <c r="B9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="24">
-        <v>5</v>
-      </c>
-      <c r="D9" s="24">
-        <v>1</v>
-      </c>
-      <c r="E9" s="24">
-        <v>1</v>
-      </c>
-      <c r="F9" s="24">
-        <v>1</v>
-      </c>
-      <c r="G9" s="24">
-        <v>1</v>
-      </c>
-      <c r="H9" s="19"/>
-      <c r="I9" s="25"/>
+      <c r="C9" s="22">
+        <v>5</v>
+      </c>
+      <c r="D9" s="22">
+        <v>1</v>
+      </c>
+      <c r="E9" s="22">
+        <v>1</v>
+      </c>
+      <c r="F9" s="22">
+        <v>1</v>
+      </c>
+      <c r="G9" s="22">
+        <v>1</v>
+      </c>
+      <c r="H9" s="17"/>
+      <c r="I9" s="23"/>
     </row>
     <row r="10" spans="1:10" ht="18" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
@@ -3189,23 +3438,23 @@
       <c r="B10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="24">
-        <v>5</v>
-      </c>
-      <c r="D10" s="24">
-        <v>1</v>
-      </c>
-      <c r="E10" s="24">
-        <v>1</v>
-      </c>
-      <c r="F10" s="24">
-        <v>1</v>
-      </c>
-      <c r="G10" s="24">
-        <v>1</v>
-      </c>
-      <c r="H10" s="19"/>
-      <c r="I10" s="25"/>
+      <c r="C10" s="22">
+        <v>5</v>
+      </c>
+      <c r="D10" s="22">
+        <v>1</v>
+      </c>
+      <c r="E10" s="22">
+        <v>1</v>
+      </c>
+      <c r="F10" s="22">
+        <v>1</v>
+      </c>
+      <c r="G10" s="22">
+        <v>1</v>
+      </c>
+      <c r="H10" s="17"/>
+      <c r="I10" s="23"/>
     </row>
     <row r="11" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
@@ -3214,23 +3463,23 @@
       <c r="B11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="24">
-        <v>5</v>
-      </c>
-      <c r="D11" s="24">
-        <v>1</v>
-      </c>
-      <c r="E11" s="24">
-        <v>1</v>
-      </c>
-      <c r="F11" s="24">
-        <v>1</v>
-      </c>
-      <c r="G11" s="24">
-        <v>1</v>
-      </c>
-      <c r="H11" s="19"/>
-      <c r="I11" s="25"/>
+      <c r="C11" s="22">
+        <v>5</v>
+      </c>
+      <c r="D11" s="22">
+        <v>1</v>
+      </c>
+      <c r="E11" s="22">
+        <v>1</v>
+      </c>
+      <c r="F11" s="22">
+        <v>1</v>
+      </c>
+      <c r="G11" s="22">
+        <v>1</v>
+      </c>
+      <c r="H11" s="17"/>
+      <c r="I11" s="23"/>
     </row>
     <row r="12" spans="1:10" ht="36" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
@@ -3239,23 +3488,23 @@
       <c r="B12" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="24">
-        <v>1</v>
-      </c>
-      <c r="D12" s="24">
-        <v>1</v>
-      </c>
-      <c r="E12" s="24">
-        <v>1</v>
-      </c>
-      <c r="F12" s="24">
-        <v>1</v>
-      </c>
-      <c r="G12" s="24">
+      <c r="C12" s="22">
+        <v>1</v>
+      </c>
+      <c r="D12" s="22">
+        <v>1</v>
+      </c>
+      <c r="E12" s="22">
+        <v>1</v>
+      </c>
+      <c r="F12" s="22">
+        <v>1</v>
+      </c>
+      <c r="G12" s="22">
         <v>2</v>
       </c>
-      <c r="H12" s="19"/>
-      <c r="I12" s="25" t="s">
+      <c r="H12" s="17"/>
+      <c r="I12" s="23" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>